<commit_message>
Update dev branch with local changes
</commit_message>
<xml_diff>
--- a/dummy_data.xlsx
+++ b/dummy_data.xlsx
@@ -20,16 +20,13 @@
     <numFmt numFmtId="164" formatCode="yyyy-mm-dd h:mm:ss"/>
     <numFmt numFmtId="165" formatCode="YYYY-MM-DD HH:MM:SS"/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="1">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -40,7 +37,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -48,21 +45,12 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
@@ -438,22 +426,22 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="inlineStr">
+      <c r="A1" t="inlineStr">
         <is>
           <t>Employee</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="B1" t="inlineStr">
         <is>
           <t>Department</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="C1" t="inlineStr">
         <is>
           <t>Sales</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="D1" t="inlineStr">
         <is>
           <t>Date</t>
         </is>
@@ -473,7 +461,7 @@
       <c r="C2" t="n">
         <v>50000</v>
       </c>
-      <c r="D2" s="2" t="n">
+      <c r="D2" s="1" t="n">
         <v>45804</v>
       </c>
     </row>
@@ -491,7 +479,7 @@
       <c r="C3" t="n">
         <v>49376</v>
       </c>
-      <c r="D3" s="2" t="n">
+      <c r="D3" s="1" t="n">
         <v>45647</v>
       </c>
     </row>
@@ -509,7 +497,7 @@
       <c r="C4" t="n">
         <v>48734</v>
       </c>
-      <c r="D4" s="2" t="n">
+      <c r="D4" s="1" t="n">
         <v>45669</v>
       </c>
     </row>
@@ -527,7 +515,7 @@
       <c r="C5" t="n">
         <v>47648</v>
       </c>
-      <c r="D5" s="2" t="n">
+      <c r="D5" s="1" t="n">
         <v>45866</v>
       </c>
     </row>
@@ -545,7 +533,7 @@
       <c r="C6" t="n">
         <v>46919</v>
       </c>
-      <c r="D6" s="2" t="n">
+      <c r="D6" s="1" t="n">
         <v>45829</v>
       </c>
     </row>
@@ -563,7 +551,7 @@
       <c r="C7" t="n">
         <v>45837</v>
       </c>
-      <c r="D7" s="2" t="n">
+      <c r="D7" s="1" t="n">
         <v>45891</v>
       </c>
     </row>
@@ -581,7 +569,7 @@
       <c r="C8" t="n">
         <v>45233</v>
       </c>
-      <c r="D8" s="2" t="n">
+      <c r="D8" s="1" t="n">
         <v>45833</v>
       </c>
     </row>
@@ -599,7 +587,7 @@
       <c r="C9" t="n">
         <v>44563</v>
       </c>
-      <c r="D9" s="2" t="n">
+      <c r="D9" s="1" t="n">
         <v>45641</v>
       </c>
     </row>
@@ -617,7 +605,7 @@
       <c r="C10" t="n">
         <v>43292</v>
       </c>
-      <c r="D10" s="2" t="n">
+      <c r="D10" s="1" t="n">
         <v>45675</v>
       </c>
     </row>
@@ -635,7 +623,7 @@
       <c r="C11" t="n">
         <v>42417</v>
       </c>
-      <c r="D11" s="2" t="n">
+      <c r="D11" s="1" t="n">
         <v>45665</v>
       </c>
     </row>
@@ -653,7 +641,7 @@
       <c r="C12" t="n">
         <v>40972</v>
       </c>
-      <c r="D12" s="2" t="n">
+      <c r="D12" s="1" t="n">
         <v>45832</v>
       </c>
     </row>
@@ -671,7 +659,7 @@
       <c r="C13" t="n">
         <v>40278</v>
       </c>
-      <c r="D13" s="2" t="n">
+      <c r="D13" s="1" t="n">
         <v>45816</v>
       </c>
     </row>
@@ -689,7 +677,7 @@
       <c r="C14" t="n">
         <v>38297</v>
       </c>
-      <c r="D14" s="2" t="n">
+      <c r="D14" s="1" t="n">
         <v>45769</v>
       </c>
     </row>
@@ -707,7 +695,7 @@
       <c r="C15" t="n">
         <v>38049</v>
       </c>
-      <c r="D15" s="2" t="n">
+      <c r="D15" s="1" t="n">
         <v>45960</v>
       </c>
     </row>
@@ -725,7 +713,7 @@
       <c r="C16" t="n">
         <v>37650</v>
       </c>
-      <c r="D16" s="2" t="n">
+      <c r="D16" s="1" t="n">
         <v>45654</v>
       </c>
     </row>
@@ -743,7 +731,7 @@
       <c r="C17" t="n">
         <v>37066</v>
       </c>
-      <c r="D17" s="2" t="n">
+      <c r="D17" s="1" t="n">
         <v>45975</v>
       </c>
     </row>
@@ -761,7 +749,7 @@
       <c r="C18" t="n">
         <v>36858</v>
       </c>
-      <c r="D18" s="2" t="n">
+      <c r="D18" s="1" t="n">
         <v>45939</v>
       </c>
     </row>
@@ -779,7 +767,7 @@
       <c r="C19" t="n">
         <v>36337</v>
       </c>
-      <c r="D19" s="2" t="n">
+      <c r="D19" s="1" t="n">
         <v>45684</v>
       </c>
     </row>
@@ -797,7 +785,7 @@
       <c r="C20" t="n">
         <v>36107</v>
       </c>
-      <c r="D20" s="2" t="n">
+      <c r="D20" s="1" t="n">
         <v>45810</v>
       </c>
     </row>
@@ -815,7 +803,7 @@
       <c r="C21" t="n">
         <v>35992</v>
       </c>
-      <c r="D21" s="2" t="n">
+      <c r="D21" s="1" t="n">
         <v>45831</v>
       </c>
     </row>
@@ -833,7 +821,7 @@
       <c r="C22" t="n">
         <v>35586</v>
       </c>
-      <c r="D22" s="2" t="n">
+      <c r="D22" s="1" t="n">
         <v>45668</v>
       </c>
     </row>
@@ -851,7 +839,7 @@
       <c r="C23" t="n">
         <v>34857</v>
       </c>
-      <c r="D23" s="2" t="n">
+      <c r="D23" s="1" t="n">
         <v>45938</v>
       </c>
     </row>
@@ -869,7 +857,7 @@
       <c r="C24" t="n">
         <v>34815</v>
       </c>
-      <c r="D24" s="2" t="n">
+      <c r="D24" s="1" t="n">
         <v>45834</v>
       </c>
     </row>
@@ -887,7 +875,7 @@
       <c r="C25" t="n">
         <v>34005</v>
       </c>
-      <c r="D25" s="2" t="n">
+      <c r="D25" s="1" t="n">
         <v>45873</v>
       </c>
     </row>
@@ -905,7 +893,7 @@
       <c r="C26" t="n">
         <v>33175</v>
       </c>
-      <c r="D26" s="2" t="n">
+      <c r="D26" s="1" t="n">
         <v>45727</v>
       </c>
     </row>
@@ -923,7 +911,7 @@
       <c r="C27" t="n">
         <v>32607</v>
       </c>
-      <c r="D27" s="2" t="n">
+      <c r="D27" s="1" t="n">
         <v>45729</v>
       </c>
     </row>
@@ -941,7 +929,7 @@
       <c r="C28" t="n">
         <v>29962</v>
       </c>
-      <c r="D28" s="2" t="n">
+      <c r="D28" s="1" t="n">
         <v>45802</v>
       </c>
     </row>
@@ -959,7 +947,7 @@
       <c r="C29" t="n">
         <v>29349</v>
       </c>
-      <c r="D29" s="2" t="n">
+      <c r="D29" s="1" t="n">
         <v>45724</v>
       </c>
     </row>
@@ -977,7 +965,7 @@
       <c r="C30" t="n">
         <v>28743</v>
       </c>
-      <c r="D30" s="2" t="n">
+      <c r="D30" s="1" t="n">
         <v>45901</v>
       </c>
     </row>
@@ -995,7 +983,7 @@
       <c r="C31" t="n">
         <v>28736</v>
       </c>
-      <c r="D31" s="2" t="n">
+      <c r="D31" s="1" t="n">
         <v>45667</v>
       </c>
     </row>
@@ -1013,7 +1001,7 @@
       <c r="C32" t="n">
         <v>28724</v>
       </c>
-      <c r="D32" s="2" t="n">
+      <c r="D32" s="1" t="n">
         <v>45727</v>
       </c>
     </row>
@@ -1031,7 +1019,7 @@
       <c r="C33" t="n">
         <v>28038</v>
       </c>
-      <c r="D33" s="2" t="n">
+      <c r="D33" s="1" t="n">
         <v>45932</v>
       </c>
     </row>
@@ -1049,7 +1037,7 @@
       <c r="C34" t="n">
         <v>27650</v>
       </c>
-      <c r="D34" s="2" t="n">
+      <c r="D34" s="1" t="n">
         <v>45733</v>
       </c>
     </row>
@@ -1067,7 +1055,7 @@
       <c r="C35" t="n">
         <v>27409</v>
       </c>
-      <c r="D35" s="2" t="n">
+      <c r="D35" s="1" t="n">
         <v>45802</v>
       </c>
     </row>
@@ -1085,7 +1073,7 @@
       <c r="C36" t="n">
         <v>26954</v>
       </c>
-      <c r="D36" s="2" t="n">
+      <c r="D36" s="1" t="n">
         <v>45656</v>
       </c>
     </row>
@@ -1103,7 +1091,7 @@
       <c r="C37" t="n">
         <v>26110</v>
       </c>
-      <c r="D37" s="2" t="n">
+      <c r="D37" s="1" t="n">
         <v>45681</v>
       </c>
     </row>
@@ -1121,7 +1109,7 @@
       <c r="C38" t="n">
         <v>25544</v>
       </c>
-      <c r="D38" s="2" t="n">
+      <c r="D38" s="1" t="n">
         <v>45966</v>
       </c>
     </row>
@@ -1139,7 +1127,7 @@
       <c r="C39" t="n">
         <v>24759</v>
       </c>
-      <c r="D39" s="2" t="n">
+      <c r="D39" s="1" t="n">
         <v>45918</v>
       </c>
     </row>
@@ -1157,7 +1145,7 @@
       <c r="C40" t="n">
         <v>24502</v>
       </c>
-      <c r="D40" s="2" t="n">
+      <c r="D40" s="1" t="n">
         <v>45887</v>
       </c>
     </row>
@@ -1175,7 +1163,7 @@
       <c r="C41" t="n">
         <v>24417</v>
       </c>
-      <c r="D41" s="2" t="n">
+      <c r="D41" s="1" t="n">
         <v>45910</v>
       </c>
     </row>
@@ -1193,7 +1181,7 @@
       <c r="C42" t="n">
         <v>24381</v>
       </c>
-      <c r="D42" s="2" t="n">
+      <c r="D42" s="1" t="n">
         <v>45711</v>
       </c>
     </row>
@@ -1211,7 +1199,7 @@
       <c r="C43" t="n">
         <v>24011</v>
       </c>
-      <c r="D43" s="2" t="n">
+      <c r="D43" s="1" t="n">
         <v>45656</v>
       </c>
     </row>
@@ -1229,7 +1217,7 @@
       <c r="C44" t="n">
         <v>23978</v>
       </c>
-      <c r="D44" s="2" t="n">
+      <c r="D44" s="1" t="n">
         <v>45759</v>
       </c>
     </row>
@@ -1247,7 +1235,7 @@
       <c r="C45" t="n">
         <v>23841</v>
       </c>
-      <c r="D45" s="2" t="n">
+      <c r="D45" s="1" t="n">
         <v>45714</v>
       </c>
     </row>
@@ -1265,7 +1253,7 @@
       <c r="C46" t="n">
         <v>22550</v>
       </c>
-      <c r="D46" s="2" t="n">
+      <c r="D46" s="1" t="n">
         <v>45749</v>
       </c>
     </row>
@@ -1283,7 +1271,7 @@
       <c r="C47" t="n">
         <v>21905</v>
       </c>
-      <c r="D47" s="2" t="n">
+      <c r="D47" s="1" t="n">
         <v>45743</v>
       </c>
     </row>
@@ -1301,7 +1289,7 @@
       <c r="C48" t="n">
         <v>21897</v>
       </c>
-      <c r="D48" s="2" t="n">
+      <c r="D48" s="1" t="n">
         <v>45684</v>
       </c>
     </row>
@@ -1319,7 +1307,7 @@
       <c r="C49" t="n">
         <v>21682</v>
       </c>
-      <c r="D49" s="2" t="n">
+      <c r="D49" s="1" t="n">
         <v>45786</v>
       </c>
     </row>
@@ -1337,7 +1325,7 @@
       <c r="C50" t="n">
         <v>21482</v>
       </c>
-      <c r="D50" s="2" t="n">
+      <c r="D50" s="1" t="n">
         <v>45832</v>
       </c>
     </row>
@@ -1355,7 +1343,7 @@
       <c r="C51" t="n">
         <v>21375</v>
       </c>
-      <c r="D51" s="2" t="n">
+      <c r="D51" s="1" t="n">
         <v>45688</v>
       </c>
     </row>
@@ -1373,7 +1361,7 @@
       <c r="C52" t="n">
         <v>20211</v>
       </c>
-      <c r="D52" s="2" t="n">
+      <c r="D52" s="1" t="n">
         <v>45859</v>
       </c>
     </row>
@@ -1391,7 +1379,7 @@
       <c r="C53" t="n">
         <v>19768</v>
       </c>
-      <c r="D53" s="2" t="n">
+      <c r="D53" s="1" t="n">
         <v>45675</v>
       </c>
     </row>
@@ -1409,7 +1397,7 @@
       <c r="C54" t="n">
         <v>19189</v>
       </c>
-      <c r="D54" s="2" t="n">
+      <c r="D54" s="1" t="n">
         <v>45801</v>
       </c>
     </row>
@@ -1427,7 +1415,7 @@
       <c r="C55" t="n">
         <v>18683</v>
       </c>
-      <c r="D55" s="2" t="n">
+      <c r="D55" s="1" t="n">
         <v>45638</v>
       </c>
     </row>
@@ -1445,7 +1433,7 @@
       <c r="C56" t="n">
         <v>18439</v>
       </c>
-      <c r="D56" s="2" t="n">
+      <c r="D56" s="1" t="n">
         <v>45862</v>
       </c>
     </row>
@@ -1463,7 +1451,7 @@
       <c r="C57" t="n">
         <v>18308</v>
       </c>
-      <c r="D57" s="2" t="n">
+      <c r="D57" s="1" t="n">
         <v>45999</v>
       </c>
     </row>
@@ -1481,7 +1469,7 @@
       <c r="C58" t="n">
         <v>18283</v>
       </c>
-      <c r="D58" s="2" t="n">
+      <c r="D58" s="1" t="n">
         <v>45663</v>
       </c>
     </row>
@@ -1499,7 +1487,7 @@
       <c r="C59" t="n">
         <v>18255</v>
       </c>
-      <c r="D59" s="2" t="n">
+      <c r="D59" s="1" t="n">
         <v>45772</v>
       </c>
     </row>
@@ -1517,7 +1505,7 @@
       <c r="C60" t="n">
         <v>17903</v>
       </c>
-      <c r="D60" s="2" t="n">
+      <c r="D60" s="1" t="n">
         <v>45654</v>
       </c>
     </row>
@@ -1535,7 +1523,7 @@
       <c r="C61" t="n">
         <v>17694</v>
       </c>
-      <c r="D61" s="2" t="n">
+      <c r="D61" s="1" t="n">
         <v>45884</v>
       </c>
     </row>
@@ -1553,7 +1541,7 @@
       <c r="C62" t="n">
         <v>17683</v>
       </c>
-      <c r="D62" s="2" t="n">
+      <c r="D62" s="1" t="n">
         <v>45944</v>
       </c>
     </row>
@@ -1571,7 +1559,7 @@
       <c r="C63" t="n">
         <v>17312</v>
       </c>
-      <c r="D63" s="2" t="n">
+      <c r="D63" s="1" t="n">
         <v>45747</v>
       </c>
     </row>
@@ -1589,7 +1577,7 @@
       <c r="C64" t="n">
         <v>16662</v>
       </c>
-      <c r="D64" s="2" t="n">
+      <c r="D64" s="1" t="n">
         <v>45835</v>
       </c>
     </row>
@@ -1607,7 +1595,7 @@
       <c r="C65" t="n">
         <v>16500</v>
       </c>
-      <c r="D65" s="2" t="n">
+      <c r="D65" s="1" t="n">
         <v>45640</v>
       </c>
     </row>
@@ -1625,7 +1613,7 @@
       <c r="C66" t="n">
         <v>15990</v>
       </c>
-      <c r="D66" s="2" t="n">
+      <c r="D66" s="1" t="n">
         <v>45817</v>
       </c>
     </row>
@@ -1643,7 +1631,7 @@
       <c r="C67" t="n">
         <v>15346</v>
       </c>
-      <c r="D67" s="2" t="n">
+      <c r="D67" s="1" t="n">
         <v>45642</v>
       </c>
     </row>
@@ -1661,7 +1649,7 @@
       <c r="C68" t="n">
         <v>15268</v>
       </c>
-      <c r="D68" s="2" t="n">
+      <c r="D68" s="1" t="n">
         <v>45979</v>
       </c>
     </row>
@@ -1679,7 +1667,7 @@
       <c r="C69" t="n">
         <v>14969</v>
       </c>
-      <c r="D69" s="2" t="n">
+      <c r="D69" s="1" t="n">
         <v>45957</v>
       </c>
     </row>
@@ -1697,7 +1685,7 @@
       <c r="C70" t="n">
         <v>14703</v>
       </c>
-      <c r="D70" s="2" t="n">
+      <c r="D70" s="1" t="n">
         <v>45797</v>
       </c>
     </row>
@@ -1715,7 +1703,7 @@
       <c r="C71" t="n">
         <v>14475</v>
       </c>
-      <c r="D71" s="2" t="n">
+      <c r="D71" s="1" t="n">
         <v>45749</v>
       </c>
     </row>
@@ -1733,7 +1721,7 @@
       <c r="C72" t="n">
         <v>13895</v>
       </c>
-      <c r="D72" s="2" t="n">
+      <c r="D72" s="1" t="n">
         <v>45666</v>
       </c>
     </row>
@@ -1751,7 +1739,7 @@
       <c r="C73" t="n">
         <v>13784</v>
       </c>
-      <c r="D73" s="2" t="n">
+      <c r="D73" s="1" t="n">
         <v>45705</v>
       </c>
     </row>
@@ -1769,7 +1757,7 @@
       <c r="C74" t="n">
         <v>13131</v>
       </c>
-      <c r="D74" s="2" t="n">
+      <c r="D74" s="1" t="n">
         <v>45932</v>
       </c>
     </row>
@@ -1787,7 +1775,7 @@
       <c r="C75" t="n">
         <v>12874</v>
       </c>
-      <c r="D75" s="2" t="n">
+      <c r="D75" s="1" t="n">
         <v>45996</v>
       </c>
     </row>
@@ -1805,7 +1793,7 @@
       <c r="C76" t="n">
         <v>12739</v>
       </c>
-      <c r="D76" s="2" t="n">
+      <c r="D76" s="1" t="n">
         <v>45940</v>
       </c>
     </row>
@@ -1823,7 +1811,7 @@
       <c r="C77" t="n">
         <v>11883</v>
       </c>
-      <c r="D77" s="2" t="n">
+      <c r="D77" s="1" t="n">
         <v>45773</v>
       </c>
     </row>
@@ -1841,7 +1829,7 @@
       <c r="C78" t="n">
         <v>11675</v>
       </c>
-      <c r="D78" s="2" t="n">
+      <c r="D78" s="1" t="n">
         <v>45904</v>
       </c>
     </row>
@@ -1859,7 +1847,7 @@
       <c r="C79" t="n">
         <v>11473</v>
       </c>
-      <c r="D79" s="2" t="n">
+      <c r="D79" s="1" t="n">
         <v>45946</v>
       </c>
     </row>
@@ -1877,7 +1865,7 @@
       <c r="C80" t="n">
         <v>11394</v>
       </c>
-      <c r="D80" s="2" t="n">
+      <c r="D80" s="1" t="n">
         <v>45815</v>
       </c>
     </row>
@@ -1895,7 +1883,7 @@
       <c r="C81" t="n">
         <v>10839</v>
       </c>
-      <c r="D81" s="2" t="n">
+      <c r="D81" s="1" t="n">
         <v>45911</v>
       </c>
     </row>
@@ -1913,7 +1901,7 @@
       <c r="C82" t="n">
         <v>10630</v>
       </c>
-      <c r="D82" s="2" t="n">
+      <c r="D82" s="1" t="n">
         <v>45953</v>
       </c>
     </row>
@@ -1931,7 +1919,7 @@
       <c r="C83" t="n">
         <v>9612</v>
       </c>
-      <c r="D83" s="2" t="n">
+      <c r="D83" s="1" t="n">
         <v>45736</v>
       </c>
     </row>
@@ -1949,7 +1937,7 @@
       <c r="C84" t="n">
         <v>9458</v>
       </c>
-      <c r="D84" s="2" t="n">
+      <c r="D84" s="1" t="n">
         <v>45794</v>
       </c>
     </row>
@@ -1967,7 +1955,7 @@
       <c r="C85" t="n">
         <v>9256</v>
       </c>
-      <c r="D85" s="2" t="n">
+      <c r="D85" s="1" t="n">
         <v>45763</v>
       </c>
     </row>
@@ -1985,7 +1973,7 @@
       <c r="C86" t="n">
         <v>8656</v>
       </c>
-      <c r="D86" s="2" t="n">
+      <c r="D86" s="1" t="n">
         <v>45736</v>
       </c>
     </row>
@@ -2003,7 +1991,7 @@
       <c r="C87" t="n">
         <v>8279</v>
       </c>
-      <c r="D87" s="2" t="n">
+      <c r="D87" s="1" t="n">
         <v>45688</v>
       </c>
     </row>
@@ -2021,7 +2009,7 @@
       <c r="C88" t="n">
         <v>7596</v>
       </c>
-      <c r="D88" s="2" t="n">
+      <c r="D88" s="1" t="n">
         <v>45948</v>
       </c>
     </row>
@@ -2039,7 +2027,7 @@
       <c r="C89" t="n">
         <v>7286</v>
       </c>
-      <c r="D89" s="2" t="n">
+      <c r="D89" s="1" t="n">
         <v>45722</v>
       </c>
     </row>
@@ -2057,7 +2045,7 @@
       <c r="C90" t="n">
         <v>6856</v>
       </c>
-      <c r="D90" s="2" t="n">
+      <c r="D90" s="1" t="n">
         <v>45784</v>
       </c>
     </row>
@@ -2075,7 +2063,7 @@
       <c r="C91" t="n">
         <v>6795</v>
       </c>
-      <c r="D91" s="2" t="n">
+      <c r="D91" s="1" t="n">
         <v>45701</v>
       </c>
     </row>
@@ -2093,7 +2081,7 @@
       <c r="C92" t="n">
         <v>6787</v>
       </c>
-      <c r="D92" s="2" t="n">
+      <c r="D92" s="1" t="n">
         <v>45876</v>
       </c>
     </row>
@@ -2111,7 +2099,7 @@
       <c r="C93" t="n">
         <v>6384</v>
       </c>
-      <c r="D93" s="2" t="n">
+      <c r="D93" s="1" t="n">
         <v>45813</v>
       </c>
     </row>
@@ -2129,7 +2117,7 @@
       <c r="C94" t="n">
         <v>6380</v>
       </c>
-      <c r="D94" s="2" t="n">
+      <c r="D94" s="1" t="n">
         <v>45973</v>
       </c>
     </row>
@@ -2147,7 +2135,7 @@
       <c r="C95" t="n">
         <v>5814</v>
       </c>
-      <c r="D95" s="2" t="n">
+      <c r="D95" s="1" t="n">
         <v>45988</v>
       </c>
     </row>
@@ -2165,7 +2153,7 @@
       <c r="C96" t="n">
         <v>5778</v>
       </c>
-      <c r="D96" s="2" t="n">
+      <c r="D96" s="1" t="n">
         <v>45699</v>
       </c>
     </row>
@@ -2183,7 +2171,7 @@
       <c r="C97" t="n">
         <v>3277</v>
       </c>
-      <c r="D97" s="2" t="n">
+      <c r="D97" s="1" t="n">
         <v>45966</v>
       </c>
     </row>
@@ -2201,7 +2189,7 @@
       <c r="C98" t="n">
         <v>2858</v>
       </c>
-      <c r="D98" s="2" t="n">
+      <c r="D98" s="1" t="n">
         <v>45972</v>
       </c>
     </row>
@@ -2219,7 +2207,7 @@
       <c r="C99" t="n">
         <v>1507</v>
       </c>
-      <c r="D99" s="2" t="n">
+      <c r="D99" s="1" t="n">
         <v>45787</v>
       </c>
     </row>
@@ -2237,7 +2225,7 @@
       <c r="C100" t="n">
         <v>1369</v>
       </c>
-      <c r="D100" s="2" t="n">
+      <c r="D100" s="1" t="n">
         <v>45968</v>
       </c>
     </row>
@@ -2255,7 +2243,7 @@
       <c r="C101" t="n">
         <v>1334</v>
       </c>
-      <c r="D101" s="2" t="n">
+      <c r="D101" s="1" t="n">
         <v>45788</v>
       </c>
     </row>

</xml_diff>